<commit_message>
working on pump data
</commit_message>
<xml_diff>
--- a/CMAP_variableMetadata_additions.xlsx
+++ b/CMAP_variableMetadata_additions.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\Dropbox\GitHub_espresso\BWrepos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D0E8286-1CED-4971-9C0E-18D8ABD7B2B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02930A57-82ED-4998-8A9F-096622321561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="4" r:id="rId1"/>
-    <sheet name="vars_meta_data" sheetId="3" r:id="rId2"/>
+    <sheet name="vars_meta_data_discrete" sheetId="3" r:id="rId2"/>
+    <sheet name="vars_meta_data_pump" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="230">
   <si>
     <t>Program</t>
   </si>
@@ -642,6 +643,75 @@
   </si>
   <si>
     <t>AE1614, AE1712, AE1819, AE1916, Bermuda Institute of Ocean Sciences, bio, biogeo, biogeochemistry, biology, BIOS, Bottle, cruise, Discrete, in situ, insitu, in-situ, North Atlantic Ocean, observation, vertical zone, stratification</t>
+  </si>
+  <si>
+    <t>Sample_ID</t>
+  </si>
+  <si>
+    <t>Cruise</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Size_fraction</t>
+  </si>
+  <si>
+    <t>Filter_type</t>
+  </si>
+  <si>
+    <t>Asp_sd</t>
+  </si>
+  <si>
+    <t>Glu_sd</t>
+  </si>
+  <si>
+    <t>HisSer</t>
+  </si>
+  <si>
+    <t>HisSer_sd</t>
+  </si>
+  <si>
+    <t>Arg_sd</t>
+  </si>
+  <si>
+    <t>Thr_sd</t>
+  </si>
+  <si>
+    <t>Gly_sd</t>
+  </si>
+  <si>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>Bala_sd</t>
+  </si>
+  <si>
+    <t>Tyr_sd</t>
+  </si>
+  <si>
+    <t>Ala_sd</t>
+  </si>
+  <si>
+    <t>GABA_sd</t>
+  </si>
+  <si>
+    <t>Met_sd</t>
+  </si>
+  <si>
+    <t>Val_sd</t>
+  </si>
+  <si>
+    <t>Phe_sd</t>
+  </si>
+  <si>
+    <t>Ile_sd</t>
+  </si>
+  <si>
+    <t>Leu_sd</t>
+  </si>
+  <si>
+    <t>Lys_sd</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1165,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="G50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I74" sqref="I74"/>
+      <selection pane="bottomRight" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3083,4 +3153,455 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1721BD-CA3E-4F68-BD4D-92695DCAE717}">
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>181</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="G8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G10" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>214</v>
+      </c>
+      <c r="G11" t="s">
+        <v>181</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="G12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>216</v>
+      </c>
+      <c r="G14" t="s">
+        <v>181</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>181</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>217</v>
+      </c>
+      <c r="G16" t="s">
+        <v>181</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
+        <v>181</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="G18" t="s">
+        <v>181</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>219</v>
+      </c>
+      <c r="G19" t="s">
+        <v>181</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G20" t="s">
+        <v>181</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" t="s">
+        <v>181</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>221</v>
+      </c>
+      <c r="G22" t="s">
+        <v>181</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G23" t="s">
+        <v>181</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="G24" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+      <c r="G26" t="s">
+        <v>181</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" t="s">
+        <v>181</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>224</v>
+      </c>
+      <c r="G28" t="s">
+        <v>181</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" t="s">
+        <v>181</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>225</v>
+      </c>
+      <c r="G30" t="s">
+        <v>181</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" t="s">
+        <v>181</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>226</v>
+      </c>
+      <c r="G32" t="s">
+        <v>181</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="G33" t="s">
+        <v>181</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>227</v>
+      </c>
+      <c r="G34" t="s">
+        <v>181</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="G35" t="s">
+        <v>181</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>228</v>
+      </c>
+      <c r="G36" t="s">
+        <v>181</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="G37" t="s">
+        <v>181</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>229</v>
+      </c>
+      <c r="G38" t="s">
+        <v>181</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
have the pieces I need
</commit_message>
<xml_diff>
--- a/CMAP_variableMetadata_additions.xlsx
+++ b/CMAP_variableMetadata_additions.xlsx
@@ -8,21 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klongnecker\Documents\Dropbox\GitHub_espresso\BWrepos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02930A57-82ED-4998-8A9F-096622321561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C71E566-F135-446C-947C-5348E4B64CD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20660" windowHeight="7880" activeTab="1" xr2:uid="{BD19A4B1-5CB6-4C93-AA6F-C3C4861757B5}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="4" r:id="rId1"/>
-    <sheet name="vars_meta_data_discrete" sheetId="3" r:id="rId2"/>
-    <sheet name="vars_meta_data_pump" sheetId="5" r:id="rId3"/>
+    <sheet name="survey_biogeochemical" sheetId="3" r:id="rId2"/>
+    <sheet name="zooscan_mocness_output" sheetId="6" r:id="rId3"/>
+    <sheet name="964826_v1_pump_poc_pon_biosscop" sheetId="7" r:id="rId4"/>
+    <sheet name="964801_v1_pump_carbohydrates_bi" sheetId="8" r:id="rId5"/>
+    <sheet name="964684_v1_amino_acids_biosscope" sheetId="9" r:id="rId6"/>
+    <sheet name="920443_v1_biosscope_in_situ_pum" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1367" uniqueCount="413">
   <si>
     <t>Program</t>
   </si>
@@ -712,6 +717,555 @@
   </si>
   <si>
     <t>Lys_sd</t>
+  </si>
+  <si>
+    <t>object_id</t>
+  </si>
+  <si>
+    <t>Particle identifier (cruise#_mocnessID_net#_sizefraction_image#)</t>
+  </si>
+  <si>
+    <t>not applicable</t>
+  </si>
+  <si>
+    <t>metadata</t>
+  </si>
+  <si>
+    <t>AE1614, AE1712, AE1819, AE1830, Bermuda Institute of Ocean Sciences, bio, biogeo, biogeochemistry, biology, BIOS, cruise, in situ, insitu, in-situ, North Atlantic Ocean, observation, zooplankton, net tows</t>
+  </si>
+  <si>
+    <t>object_date</t>
+  </si>
+  <si>
+    <t>Date of Collection in format yyyymmdd</t>
+  </si>
+  <si>
+    <t>object_time</t>
+  </si>
+  <si>
+    <t>Time of Collection in format hhmmss</t>
+  </si>
+  <si>
+    <t>Datetime (UTC) of Collection in ISO 8601 format yyyy-mm-ddTHH:MMZ.</t>
+  </si>
+  <si>
+    <t>%Y-%m-%dT%H:%M:%SZ</t>
+  </si>
+  <si>
+    <t>object_depth_min</t>
+  </si>
+  <si>
+    <t>Minimum depth of net collection</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>object_depth_max</t>
+  </si>
+  <si>
+    <t>Maximum depth of net collection</t>
+  </si>
+  <si>
+    <t>object_annotation_hierarchy</t>
+  </si>
+  <si>
+    <t>Taxonomic classification (predicted except for AE1712 which was validated)</t>
+  </si>
+  <si>
+    <t>biology</t>
+  </si>
+  <si>
+    <t>object_area</t>
+  </si>
+  <si>
+    <t>Object area in pixels</t>
+  </si>
+  <si>
+    <t>pix^2</t>
+  </si>
+  <si>
+    <t>object_major</t>
+  </si>
+  <si>
+    <t>Object major axis length in pixels</t>
+  </si>
+  <si>
+    <t>pix</t>
+  </si>
+  <si>
+    <t>object_minor</t>
+  </si>
+  <si>
+    <t>Object minor axis length in pixels</t>
+  </si>
+  <si>
+    <t>object_feret</t>
+  </si>
+  <si>
+    <t>Object Maximum feret diameter, i.e., the longest distance between any two points along the object boundary in pixels</t>
+  </si>
+  <si>
+    <t>object_esd</t>
+  </si>
+  <si>
+    <t>Object Equivalent Spherical Diameter</t>
+  </si>
+  <si>
+    <t>sample_tot_vol</t>
+  </si>
+  <si>
+    <t>Volume filtered</t>
+  </si>
+  <si>
+    <t>m^3</t>
+  </si>
+  <si>
+    <t>acq_sub_part</t>
+  </si>
+  <si>
+    <t>number of splits</t>
+  </si>
+  <si>
+    <t>Internal sample ID</t>
+  </si>
+  <si>
+    <t>BIOSSCOPE cruise identifier</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>Particle size range for water fraction</t>
+  </si>
+  <si>
+    <t>micrometers (um)</t>
+  </si>
+  <si>
+    <t>Filter type used for particle fraction (Nitex, GF/C ,GF75)</t>
+  </si>
+  <si>
+    <t>nanomoles carbon per liter</t>
+  </si>
+  <si>
+    <t>standard deviation of Aspartic Acid concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Glutamic Acid concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Histidine+Serine amino acid concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Arginine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Threonine concenctration</t>
+  </si>
+  <si>
+    <t>standard deviation of Glycine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Beta-alanine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Tyrosine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Alanine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Gamma-aminobutyric acid concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Methionine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Valine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Phenylalanine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Isoleucine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Leucine concentration</t>
+  </si>
+  <si>
+    <t>standard deviation of Lysine concentration</t>
+  </si>
+  <si>
+    <t>Date of sample collection</t>
+  </si>
+  <si>
+    <t>biogeochemistry</t>
+  </si>
+  <si>
+    <t>Fucose</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Fucose</t>
+  </si>
+  <si>
+    <t>nanomoles carbon per liter (nmol C/L)</t>
+  </si>
+  <si>
+    <t>Fucose_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Fucose concentration</t>
+  </si>
+  <si>
+    <t>Rhamnose</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Rhamnose</t>
+  </si>
+  <si>
+    <t>Rhamnose_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Rhamnose concentration</t>
+  </si>
+  <si>
+    <t>Galactosamine</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Galactosamine</t>
+  </si>
+  <si>
+    <t>Galactosamine_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Galactosamine concentration</t>
+  </si>
+  <si>
+    <t>Arabinose</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Arabinose</t>
+  </si>
+  <si>
+    <t>Arabinose_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Arabinose concentration</t>
+  </si>
+  <si>
+    <t>Glucosamine</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Glucosamine</t>
+  </si>
+  <si>
+    <t>Glucosamine_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Glucosamine concentration</t>
+  </si>
+  <si>
+    <t>Galactose</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Galactose</t>
+  </si>
+  <si>
+    <t>Galactose_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Galactose concentration</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Glucose</t>
+  </si>
+  <si>
+    <t>Glucose_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Glucose concentration</t>
+  </si>
+  <si>
+    <t>MannoseXylose</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Mannose+Xylose</t>
+  </si>
+  <si>
+    <t>MannoseXylose_sd</t>
+  </si>
+  <si>
+    <t>Ribose</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Ribose</t>
+  </si>
+  <si>
+    <t>Ribose_sd</t>
+  </si>
+  <si>
+    <t>MurAc</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Muramic acid</t>
+  </si>
+  <si>
+    <t>MurAc_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Muramic acid concentration</t>
+  </si>
+  <si>
+    <t>GalURA</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Galacturonic acid</t>
+  </si>
+  <si>
+    <t>GalURA_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Galacturonic acid concentration</t>
+  </si>
+  <si>
+    <t>GlcURA</t>
+  </si>
+  <si>
+    <t>Carbohydrate monomer average concentration: Glucuronic acid</t>
+  </si>
+  <si>
+    <t>GlcURA_sd</t>
+  </si>
+  <si>
+    <t>Standard deviation of Glucuronic acid concentration</t>
+  </si>
+  <si>
+    <t>Depth_sd</t>
+  </si>
+  <si>
+    <t>standard deviation of the depth</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>micrograms per liter (ug/L)</t>
+  </si>
+  <si>
+    <t>PN_sd</t>
+  </si>
+  <si>
+    <t>standard deviation for bulk particulate nitrogen</t>
+  </si>
+  <si>
+    <t>POC_sd</t>
+  </si>
+  <si>
+    <t>standard deviation for bulk particulate organic carbon</t>
+  </si>
+  <si>
+    <t>CN_acnonac</t>
+  </si>
+  <si>
+    <t>Carbon to nitrogen ratio of acidified POC to non-acidified PN</t>
+  </si>
+  <si>
+    <t>mole to mole (mol/mol)</t>
+  </si>
+  <si>
+    <t>CN_acnonac_sd</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>size_fraction_um</t>
+  </si>
+  <si>
+    <t>particle size range for water fraction</t>
+  </si>
+  <si>
+    <t>split_type</t>
+  </si>
+  <si>
+    <t>total_phytol_from_chlorophyll_concentration_ng_L</t>
+  </si>
+  <si>
+    <t>phytol concentration</t>
+  </si>
+  <si>
+    <t>nanograms per liter (ng/L)</t>
+  </si>
+  <si>
+    <t>phytol_concentration_sd_ng_L</t>
+  </si>
+  <si>
+    <t>phytol concentration standard deviation</t>
+  </si>
+  <si>
+    <t>d13C_phytol_corrected_value_per_mil</t>
+  </si>
+  <si>
+    <t>stable carbon isotope composition of phytol</t>
+  </si>
+  <si>
+    <t>per mil</t>
+  </si>
+  <si>
+    <t>d13C_phytol_sd_per_mil</t>
+  </si>
+  <si>
+    <t>stable carbon isotope composition of phytol standard deviation</t>
+  </si>
+  <si>
+    <t>d13C_POC_per_mil</t>
+  </si>
+  <si>
+    <t>stable carbon isotope composition of bulk particulate organic carbon</t>
+  </si>
+  <si>
+    <t>d13C_POC_sd_per_mil</t>
+  </si>
+  <si>
+    <t>stable carbon isotope composition of bulk particulate organic carbon standard deviation</t>
+  </si>
+  <si>
+    <t>POC_concentration_ug_L</t>
+  </si>
+  <si>
+    <t>bulk particulate organic carbon</t>
+  </si>
+  <si>
+    <t>d13C_THAA_per_mil</t>
+  </si>
+  <si>
+    <t>d13C values of total hydrolysable amino acids</t>
+  </si>
+  <si>
+    <t>d13C_THAA_sd_per_mil</t>
+  </si>
+  <si>
+    <t>d13C THAA standard deviation</t>
+  </si>
+  <si>
+    <t>TP_from_d15N_AA</t>
+  </si>
+  <si>
+    <t>TP_sd</t>
+  </si>
+  <si>
+    <t>Trophic Position (TP) standard deviation</t>
+  </si>
+  <si>
+    <t>Date (local, Bermuda) of sample collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POM trophic position (TP) </t>
+  </si>
+  <si>
+    <t>calculated from measured d15N values of glutamic acid+glutamine (Glx) and phenylalanine (Phe) as in Chikaraishi et al. (2009): TP = (d15NGlx - d15NPhe - 3.4)/7.6 + 1 . TP propagated uncertainty was calculated as in Jarman et al. (2017).</t>
+  </si>
+  <si>
+    <t>One filter split was prepared per sample, and three aliquots from the final prepared solution were analyzed (triplicate injections).</t>
+  </si>
+  <si>
+    <t>average amino acid concentration: Aspartic Acid</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Glutamic Acid</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Histidine+Serine</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Arginine</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Threonine</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Phenylalanine</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Isoleucine</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Leucine</t>
+  </si>
+  <si>
+    <t>average amino acid concentration:  Lysine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average amino acid concentration:  Glycine  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">average amino acid concentration:  Beta-alanine  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">average amino acid concentration:  Tyrosine  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">average amino acid concentration:  Alanine  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">average amino acid concentration:  Gamma-aminobutyric acid  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">average amino acid concentration:  Methionine  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">average amino acid concentration:  Valine  </t>
+  </si>
+  <si>
+    <t>AE2114, AE2123, Bermuda Institute of Ocean Sciences, bio, biogeo, biogeochemistry, biology, BIOS, McLane pump, cruise, in situ, insitu, in-situ, North Atlantic Ocean, observation</t>
+  </si>
+  <si>
+    <t>AE1819, AE1916, AE2114, AE2123, AE2213, AE2315,  Bermuda Institute of Ocean Sciences, bio, biogeo, biogeochemistry, biology, BIOS, McLane pump, cruise, in situ, insitu, in-situ, North Atlantic Ocean, observation</t>
+  </si>
+  <si>
+    <t>Date of sampling</t>
+  </si>
+  <si>
+    <t>PN; average bulk particulate nitrogen</t>
+  </si>
+  <si>
+    <t>one sample filter analyzed, replicate blanks used to incorporate uncertainty</t>
+  </si>
+  <si>
+    <t>POC; average bulk particulate organic carbon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter type used for particle fraction </t>
+  </si>
+  <si>
+    <t>Nitex, GF/C ,GF75</t>
+  </si>
+  <si>
+    <t>standard deviation of CN ratio</t>
+  </si>
+  <si>
+    <t>propagated error from POC and PN</t>
+  </si>
+  <si>
+    <t>AE1819, AE1916, AE2114, AE2123, AE2213, AE2315, Bermuda Institute of Ocean Sciences, bio, biogeo, biogeochemistry, biology, BIOS, McLane pump, cruise, in situ, insitu, in-situ, North Atlantic Ocean, observation</t>
+  </si>
+  <si>
+    <t>Standard deviation of Mannose+Xylose concentration</t>
+  </si>
+  <si>
+    <t>Standard deviation of Ribose concentration</t>
+  </si>
+  <si>
+    <t>Condition under which filter was stored and split into fractions for analysis</t>
+  </si>
+  <si>
+    <t>frozen or freeze dried</t>
+  </si>
+  <si>
+    <t>AE1819, Bermuda Institute of Ocean Sciences, bio, biogeo, biogeochemistry, biology, BIOS, McLane pump, cruise, in situ, insitu, in-situ, North Atlantic Ocean, observation</t>
   </si>
 </sst>
 </file>
@@ -778,13 +1332,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1129,6 +1684,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1161,11 +1717,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="G50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="I50" sqref="I50"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3156,22 +3715,2704 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1721BD-CA3E-4F68-BD4D-92695DCAE717}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8991815-1D31-4593-9F80-5C6680CDDD79}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.6328125" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" t="s">
+        <v>243</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+      <c r="D8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" t="s">
+        <v>248</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>252</v>
+      </c>
+      <c r="B10" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" t="s">
+        <v>256</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" t="s">
+        <v>248</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+      <c r="D12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" t="s">
+        <v>248</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B13" t="s">
+        <v>260</v>
+      </c>
+      <c r="D13" t="s">
+        <v>254</v>
+      </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" t="s">
+        <v>248</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>261</v>
+      </c>
+      <c r="B14" t="s">
+        <v>262</v>
+      </c>
+      <c r="D14" t="s">
+        <v>263</v>
+      </c>
+      <c r="E14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" t="s">
+        <v>233</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>264</v>
+      </c>
+      <c r="B15" t="s">
+        <v>265</v>
+      </c>
+      <c r="D15" t="s">
+        <v>265</v>
+      </c>
+      <c r="E15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" t="s">
+        <v>233</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2697E4D0-01FA-4D17-8BBE-F5E7FE4EFC08}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="61.54296875" customWidth="1"/>
+    <col min="3" max="6" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>398</v>
+      </c>
+      <c r="J6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>340</v>
+      </c>
+      <c r="B8" t="s">
+        <v>400</v>
+      </c>
+      <c r="D8" t="s">
+        <v>341</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" t="s">
+        <v>181</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>398</v>
+      </c>
+      <c r="J8" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>342</v>
+      </c>
+      <c r="B9" t="s">
+        <v>343</v>
+      </c>
+      <c r="D9" t="s">
+        <v>341</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" t="s">
+        <v>181</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>402</v>
+      </c>
+      <c r="D10" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" t="s">
+        <v>181</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>398</v>
+      </c>
+      <c r="J10" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>344</v>
+      </c>
+      <c r="B11" t="s">
+        <v>345</v>
+      </c>
+      <c r="D11" t="s">
+        <v>341</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" t="s">
+        <v>181</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" t="s">
+        <v>347</v>
+      </c>
+      <c r="D12" t="s">
+        <v>348</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13" t="s">
+        <v>405</v>
+      </c>
+      <c r="D13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>398</v>
+      </c>
+      <c r="J13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7099CAE1-6CB4-4BAE-923C-2C4D2F549912}">
+  <dimension ref="A1:J30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.7265625" customWidth="1"/>
+    <col min="2" max="2" width="53.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>397</v>
+      </c>
+      <c r="J6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" t="s">
+        <v>290</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" t="s">
+        <v>295</v>
+      </c>
+      <c r="D8" t="s">
+        <v>293</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" t="s">
+        <v>290</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" t="s">
+        <v>297</v>
+      </c>
+      <c r="D9" t="s">
+        <v>293</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" t="s">
+        <v>290</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" t="s">
+        <v>299</v>
+      </c>
+      <c r="D10" t="s">
+        <v>293</v>
+      </c>
+      <c r="E10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" t="s">
+        <v>301</v>
+      </c>
+      <c r="D11" t="s">
+        <v>293</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" t="s">
+        <v>290</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B12" t="s">
+        <v>303</v>
+      </c>
+      <c r="D12" t="s">
+        <v>293</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" t="s">
+        <v>290</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" t="s">
+        <v>305</v>
+      </c>
+      <c r="D13" t="s">
+        <v>293</v>
+      </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" t="s">
+        <v>290</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" t="s">
+        <v>307</v>
+      </c>
+      <c r="D14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" t="s">
+        <v>309</v>
+      </c>
+      <c r="D15" t="s">
+        <v>293</v>
+      </c>
+      <c r="E15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" t="s">
+        <v>290</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>310</v>
+      </c>
+      <c r="B16" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" t="s">
+        <v>293</v>
+      </c>
+      <c r="E16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" t="s">
+        <v>290</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" t="s">
+        <v>313</v>
+      </c>
+      <c r="D17" t="s">
+        <v>293</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G17" t="s">
+        <v>290</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>314</v>
+      </c>
+      <c r="B18" t="s">
+        <v>315</v>
+      </c>
+      <c r="D18" t="s">
+        <v>293</v>
+      </c>
+      <c r="E18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" t="s">
+        <v>290</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" t="s">
+        <v>317</v>
+      </c>
+      <c r="D19" t="s">
+        <v>293</v>
+      </c>
+      <c r="E19" t="s">
+        <v>175</v>
+      </c>
+      <c r="F19" t="s">
+        <v>175</v>
+      </c>
+      <c r="G19" t="s">
+        <v>290</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>318</v>
+      </c>
+      <c r="B20" t="s">
+        <v>319</v>
+      </c>
+      <c r="D20" t="s">
+        <v>293</v>
+      </c>
+      <c r="E20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" t="s">
+        <v>175</v>
+      </c>
+      <c r="G20" t="s">
+        <v>290</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>320</v>
+      </c>
+      <c r="B21" t="s">
+        <v>321</v>
+      </c>
+      <c r="D21" t="s">
+        <v>293</v>
+      </c>
+      <c r="E21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" t="s">
+        <v>290</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>322</v>
+      </c>
+      <c r="B22" t="s">
+        <v>408</v>
+      </c>
+      <c r="D22" t="s">
+        <v>293</v>
+      </c>
+      <c r="E22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" t="s">
+        <v>175</v>
+      </c>
+      <c r="G22" t="s">
+        <v>290</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>323</v>
+      </c>
+      <c r="B23" t="s">
+        <v>324</v>
+      </c>
+      <c r="D23" t="s">
+        <v>293</v>
+      </c>
+      <c r="E23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" t="s">
+        <v>290</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>325</v>
+      </c>
+      <c r="B24" t="s">
+        <v>409</v>
+      </c>
+      <c r="D24" t="s">
+        <v>293</v>
+      </c>
+      <c r="E24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" t="s">
+        <v>290</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>326</v>
+      </c>
+      <c r="B25" t="s">
+        <v>327</v>
+      </c>
+      <c r="D25" t="s">
+        <v>293</v>
+      </c>
+      <c r="E25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" t="s">
+        <v>290</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>328</v>
+      </c>
+      <c r="B26" t="s">
+        <v>329</v>
+      </c>
+      <c r="D26" t="s">
+        <v>293</v>
+      </c>
+      <c r="E26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" t="s">
+        <v>290</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>330</v>
+      </c>
+      <c r="B27" t="s">
+        <v>331</v>
+      </c>
+      <c r="D27" t="s">
+        <v>293</v>
+      </c>
+      <c r="E27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" t="s">
+        <v>175</v>
+      </c>
+      <c r="G27" t="s">
+        <v>290</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>332</v>
+      </c>
+      <c r="B28" t="s">
+        <v>333</v>
+      </c>
+      <c r="D28" t="s">
+        <v>293</v>
+      </c>
+      <c r="E28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F28" t="s">
+        <v>175</v>
+      </c>
+      <c r="G28" t="s">
+        <v>290</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>334</v>
+      </c>
+      <c r="B29" t="s">
+        <v>335</v>
+      </c>
+      <c r="D29" t="s">
+        <v>293</v>
+      </c>
+      <c r="E29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="s">
+        <v>175</v>
+      </c>
+      <c r="G29" t="s">
+        <v>290</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>336</v>
+      </c>
+      <c r="B30" t="s">
+        <v>337</v>
+      </c>
+      <c r="D30" t="s">
+        <v>293</v>
+      </c>
+      <c r="E30" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" t="s">
+        <v>290</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB974035-0AE0-4708-B122-4F86D23A7186}">
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" t="s">
+        <v>233</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>381</v>
+      </c>
+      <c r="D7" t="s">
+        <v>272</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G7" t="s">
+        <v>290</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>397</v>
+      </c>
+      <c r="J7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D8" t="s">
+        <v>272</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" t="s">
+        <v>290</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>382</v>
+      </c>
+      <c r="D9" t="s">
+        <v>272</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" t="s">
+        <v>290</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>397</v>
+      </c>
+      <c r="J9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B10" t="s">
+        <v>274</v>
+      </c>
+      <c r="D10" t="s">
+        <v>272</v>
+      </c>
+      <c r="E10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" t="s">
+        <v>290</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11" t="s">
+        <v>383</v>
+      </c>
+      <c r="D11" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>175</v>
+      </c>
+      <c r="G11" t="s">
+        <v>290</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>397</v>
+      </c>
+      <c r="J11" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G12" t="s">
+        <v>290</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>384</v>
+      </c>
+      <c r="D13" t="s">
+        <v>272</v>
+      </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" t="s">
+        <v>290</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>397</v>
+      </c>
+      <c r="J13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>216</v>
+      </c>
+      <c r="B14" t="s">
+        <v>276</v>
+      </c>
+      <c r="D14" t="s">
+        <v>272</v>
+      </c>
+      <c r="E14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" t="s">
+        <v>290</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>385</v>
+      </c>
+      <c r="D15" t="s">
+        <v>272</v>
+      </c>
+      <c r="E15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" t="s">
+        <v>290</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>397</v>
+      </c>
+      <c r="J15" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>217</v>
+      </c>
+      <c r="B16" t="s">
+        <v>277</v>
+      </c>
+      <c r="D16" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" t="s">
+        <v>290</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>390</v>
+      </c>
+      <c r="D17" t="s">
+        <v>272</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" t="s">
+        <v>175</v>
+      </c>
+      <c r="G17" t="s">
+        <v>290</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>397</v>
+      </c>
+      <c r="J17" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
+        <v>278</v>
+      </c>
+      <c r="D18" t="s">
+        <v>272</v>
+      </c>
+      <c r="E18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F18" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" t="s">
+        <v>290</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" t="s">
+        <v>391</v>
+      </c>
+      <c r="D19" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" t="s">
+        <v>175</v>
+      </c>
+      <c r="F19" t="s">
+        <v>175</v>
+      </c>
+      <c r="G19" t="s">
+        <v>290</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>397</v>
+      </c>
+      <c r="J19" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" t="s">
+        <v>279</v>
+      </c>
+      <c r="D20" t="s">
+        <v>272</v>
+      </c>
+      <c r="E20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" t="s">
+        <v>175</v>
+      </c>
+      <c r="G20" t="s">
+        <v>290</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>392</v>
+      </c>
+      <c r="D21" t="s">
+        <v>272</v>
+      </c>
+      <c r="E21" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" t="s">
+        <v>290</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>397</v>
+      </c>
+      <c r="J21" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B22" t="s">
+        <v>280</v>
+      </c>
+      <c r="D22" t="s">
+        <v>272</v>
+      </c>
+      <c r="E22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" t="s">
+        <v>175</v>
+      </c>
+      <c r="G22" t="s">
+        <v>290</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>393</v>
+      </c>
+      <c r="D23" t="s">
+        <v>272</v>
+      </c>
+      <c r="E23" t="s">
+        <v>175</v>
+      </c>
+      <c r="F23" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" t="s">
+        <v>290</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>397</v>
+      </c>
+      <c r="J23" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" t="s">
+        <v>281</v>
+      </c>
+      <c r="D24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E24" t="s">
+        <v>175</v>
+      </c>
+      <c r="F24" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" t="s">
+        <v>290</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>394</v>
+      </c>
+      <c r="D25" t="s">
+        <v>272</v>
+      </c>
+      <c r="E25" t="s">
+        <v>175</v>
+      </c>
+      <c r="F25" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" t="s">
+        <v>290</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25" t="s">
+        <v>397</v>
+      </c>
+      <c r="J25" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" t="s">
+        <v>282</v>
+      </c>
+      <c r="D26" t="s">
+        <v>272</v>
+      </c>
+      <c r="E26" t="s">
+        <v>175</v>
+      </c>
+      <c r="F26" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" t="s">
+        <v>290</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>395</v>
+      </c>
+      <c r="D27" t="s">
+        <v>272</v>
+      </c>
+      <c r="E27" t="s">
+        <v>175</v>
+      </c>
+      <c r="F27" t="s">
+        <v>175</v>
+      </c>
+      <c r="G27" t="s">
+        <v>290</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>397</v>
+      </c>
+      <c r="J27" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B28" t="s">
+        <v>283</v>
+      </c>
+      <c r="D28" t="s">
+        <v>272</v>
+      </c>
+      <c r="E28" t="s">
+        <v>175</v>
+      </c>
+      <c r="F28" t="s">
+        <v>175</v>
+      </c>
+      <c r="G28" t="s">
+        <v>290</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" t="s">
+        <v>396</v>
+      </c>
+      <c r="D29" t="s">
+        <v>272</v>
+      </c>
+      <c r="E29" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" t="s">
+        <v>175</v>
+      </c>
+      <c r="G29" t="s">
+        <v>290</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>397</v>
+      </c>
+      <c r="J29" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>225</v>
+      </c>
+      <c r="B30" t="s">
+        <v>284</v>
+      </c>
+      <c r="D30" t="s">
+        <v>272</v>
+      </c>
+      <c r="E30" t="s">
+        <v>175</v>
+      </c>
+      <c r="F30" t="s">
+        <v>175</v>
+      </c>
+      <c r="G30" t="s">
+        <v>290</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>386</v>
+      </c>
+      <c r="D31" t="s">
+        <v>272</v>
+      </c>
+      <c r="E31" t="s">
+        <v>175</v>
+      </c>
+      <c r="F31" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" t="s">
+        <v>290</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>397</v>
+      </c>
+      <c r="J31" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" t="s">
+        <v>285</v>
+      </c>
+      <c r="D32" t="s">
+        <v>272</v>
+      </c>
+      <c r="E32" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" t="s">
+        <v>290</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>387</v>
+      </c>
+      <c r="D33" t="s">
+        <v>272</v>
+      </c>
+      <c r="E33" t="s">
+        <v>175</v>
+      </c>
+      <c r="F33" t="s">
+        <v>175</v>
+      </c>
+      <c r="G33" t="s">
+        <v>290</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>397</v>
+      </c>
+      <c r="J33" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" t="s">
+        <v>286</v>
+      </c>
+      <c r="D34" t="s">
+        <v>272</v>
+      </c>
+      <c r="E34" t="s">
+        <v>175</v>
+      </c>
+      <c r="F34" t="s">
+        <v>175</v>
+      </c>
+      <c r="G34" t="s">
+        <v>290</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>388</v>
+      </c>
+      <c r="D35" t="s">
+        <v>272</v>
+      </c>
+      <c r="E35" t="s">
+        <v>175</v>
+      </c>
+      <c r="F35" t="s">
+        <v>175</v>
+      </c>
+      <c r="G35" t="s">
+        <v>290</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>397</v>
+      </c>
+      <c r="J35" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>228</v>
+      </c>
+      <c r="B36" t="s">
+        <v>287</v>
+      </c>
+      <c r="D36" t="s">
+        <v>272</v>
+      </c>
+      <c r="E36" t="s">
+        <v>175</v>
+      </c>
+      <c r="F36" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" t="s">
+        <v>290</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" t="s">
+        <v>389</v>
+      </c>
+      <c r="D37" t="s">
+        <v>272</v>
+      </c>
+      <c r="E37" t="s">
+        <v>175</v>
+      </c>
+      <c r="F37" t="s">
+        <v>175</v>
+      </c>
+      <c r="G37" t="s">
+        <v>290</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>397</v>
+      </c>
+      <c r="J37" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>229</v>
+      </c>
+      <c r="B38" t="s">
+        <v>288</v>
+      </c>
+      <c r="D38" t="s">
+        <v>272</v>
+      </c>
+      <c r="E38" t="s">
+        <v>175</v>
+      </c>
+      <c r="F38" t="s">
+        <v>175</v>
+      </c>
+      <c r="G38" t="s">
+        <v>290</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>397</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D41A31BB-44F9-4FF4-A103-F42535BD8AD4}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="35.26953125" customWidth="1"/>
+    <col min="2" max="2" width="56.7265625" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.453125" bestFit="1" customWidth="1"/>
@@ -3211,47 +6452,152 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>350</v>
+      </c>
+      <c r="B2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" t="s">
+        <v>182</v>
       </c>
       <c r="H2">
         <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>208</v>
       </c>
+      <c r="B3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" t="s">
+        <v>175</v>
+      </c>
+      <c r="F3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" t="s">
+        <v>182</v>
+      </c>
       <c r="H3">
         <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>209</v>
       </c>
+      <c r="B4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" t="s">
+        <v>182</v>
+      </c>
       <c r="H4">
         <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>351</v>
+      </c>
+      <c r="B5" t="s">
+        <v>352</v>
+      </c>
+      <c r="D5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G5" t="s">
+        <v>182</v>
       </c>
       <c r="H5">
         <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>211</v>
+        <v>353</v>
+      </c>
+      <c r="B6" t="s">
+        <v>410</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G6" t="s">
+        <v>182</v>
       </c>
       <c r="H6">
         <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>412</v>
+      </c>
+      <c r="J6" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>354</v>
+      </c>
+      <c r="B7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D7" t="s">
+        <v>356</v>
+      </c>
+      <c r="E7" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" t="s">
+        <v>175</v>
       </c>
       <c r="G7" t="s">
         <v>181</v>
@@ -3259,10 +6605,25 @@
       <c r="H7">
         <v>1</v>
       </c>
+      <c r="I7" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>212</v>
+        <v>357</v>
+      </c>
+      <c r="B8" t="s">
+        <v>358</v>
+      </c>
+      <c r="D8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E8" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" t="s">
+        <v>175</v>
       </c>
       <c r="G8" t="s">
         <v>181</v>
@@ -3270,10 +6631,25 @@
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>50</v>
+        <v>359</v>
+      </c>
+      <c r="B9" t="s">
+        <v>360</v>
+      </c>
+      <c r="D9" t="s">
+        <v>361</v>
+      </c>
+      <c r="E9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" t="s">
+        <v>175</v>
       </c>
       <c r="G9" t="s">
         <v>181</v>
@@ -3281,10 +6657,25 @@
       <c r="H9">
         <v>1</v>
       </c>
+      <c r="I9" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>362</v>
+      </c>
+      <c r="B10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D10" t="s">
+        <v>361</v>
+      </c>
+      <c r="E10" t="s">
+        <v>175</v>
+      </c>
+      <c r="F10" t="s">
+        <v>175</v>
       </c>
       <c r="G10" t="s">
         <v>181</v>
@@ -3292,10 +6683,25 @@
       <c r="H10">
         <v>0</v>
       </c>
+      <c r="I10" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>214</v>
+        <v>364</v>
+      </c>
+      <c r="B11" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" t="s">
+        <v>361</v>
+      </c>
+      <c r="E11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F11" t="s">
+        <v>175</v>
       </c>
       <c r="G11" t="s">
         <v>181</v>
@@ -3303,10 +6709,25 @@
       <c r="H11">
         <v>1</v>
       </c>
+      <c r="I11" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>215</v>
+        <v>366</v>
+      </c>
+      <c r="B12" t="s">
+        <v>367</v>
+      </c>
+      <c r="D12" t="s">
+        <v>361</v>
+      </c>
+      <c r="E12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F12" t="s">
+        <v>175</v>
       </c>
       <c r="G12" t="s">
         <v>181</v>
@@ -3314,10 +6735,25 @@
       <c r="H12">
         <v>0</v>
       </c>
+      <c r="I12" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>46</v>
+        <v>368</v>
+      </c>
+      <c r="B13" t="s">
+        <v>369</v>
+      </c>
+      <c r="D13" t="s">
+        <v>341</v>
+      </c>
+      <c r="E13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>175</v>
       </c>
       <c r="G13" t="s">
         <v>181</v>
@@ -3325,280 +6761,115 @@
       <c r="H13">
         <v>1</v>
       </c>
+      <c r="I13" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>216</v>
+        <v>370</v>
+      </c>
+      <c r="B14" t="s">
+        <v>371</v>
+      </c>
+      <c r="D14" t="s">
+        <v>361</v>
+      </c>
+      <c r="E14" t="s">
+        <v>175</v>
+      </c>
+      <c r="F14" t="s">
+        <v>175</v>
       </c>
       <c r="G14" t="s">
         <v>181</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>372</v>
+      </c>
+      <c r="B15" t="s">
+        <v>373</v>
+      </c>
+      <c r="D15" t="s">
+        <v>361</v>
+      </c>
+      <c r="E15" t="s">
+        <v>175</v>
+      </c>
+      <c r="F15" t="s">
+        <v>175</v>
       </c>
       <c r="G15" t="s">
         <v>181</v>
       </c>
       <c r="H15">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>412</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>217</v>
+        <v>374</v>
+      </c>
+      <c r="B16" t="s">
+        <v>378</v>
+      </c>
+      <c r="D16" t="s">
+        <v>159</v>
+      </c>
+      <c r="E16" t="s">
+        <v>175</v>
+      </c>
+      <c r="F16" t="s">
+        <v>175</v>
       </c>
       <c r="G16" t="s">
         <v>181</v>
       </c>
       <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>412</v>
+      </c>
+      <c r="J16" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>375</v>
+      </c>
+      <c r="B17" t="s">
+        <v>376</v>
+      </c>
+      <c r="D17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F17" t="s">
+        <v>175</v>
       </c>
       <c r="G17" t="s">
         <v>181</v>
       </c>
       <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>218</v>
-      </c>
-      <c r="G18" t="s">
-        <v>181</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>219</v>
-      </c>
-      <c r="G19" t="s">
-        <v>181</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>220</v>
-      </c>
-      <c r="G20" t="s">
-        <v>181</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="G21" t="s">
-        <v>181</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>221</v>
-      </c>
-      <c r="G22" t="s">
-        <v>181</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="G23" t="s">
-        <v>181</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>222</v>
-      </c>
-      <c r="G24" t="s">
-        <v>181</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" t="s">
-        <v>181</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>223</v>
-      </c>
-      <c r="G26" t="s">
-        <v>181</v>
-      </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>56</v>
-      </c>
-      <c r="G27" t="s">
-        <v>181</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>224</v>
-      </c>
-      <c r="G28" t="s">
-        <v>181</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" t="s">
-        <v>181</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>225</v>
-      </c>
-      <c r="G30" t="s">
-        <v>181</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>57</v>
-      </c>
-      <c r="G31" t="s">
-        <v>181</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>226</v>
-      </c>
-      <c r="G32" t="s">
-        <v>181</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33" t="s">
-        <v>181</v>
-      </c>
-      <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>227</v>
-      </c>
-      <c r="G34" t="s">
-        <v>181</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>54</v>
-      </c>
-      <c r="G35" t="s">
-        <v>181</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>228</v>
-      </c>
-      <c r="G36" t="s">
-        <v>181</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>55</v>
-      </c>
-      <c r="G37" t="s">
-        <v>181</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>229</v>
-      </c>
-      <c r="G38" t="s">
-        <v>181</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>